<commit_message>
Adding my work files
</commit_message>
<xml_diff>
--- a/df_corr.xlsx
+++ b/df_corr.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coursework\UCI-IRV-DATA-PT-11-2019 - Copy\Project_1_Team_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD2F1D8-86AF-4226-A625-E09C52E5E3D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6008AEF-7A13-4921-90C5-2F7D3D07329B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="df_corr" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Salary" sheetId="2" r:id="rId2"/>
+    <sheet name="Rank" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="30">
   <si>
     <t>YEAR</t>
   </si>
@@ -674,6 +675,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Correlation between salaries for</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 324 players and all stats.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -715,7 +746,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Salary!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -736,7 +767,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$AC$1</c:f>
+              <c:f>Salary!$B$1:$AC$1</c:f>
               <c:strCache>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
@@ -828,7 +859,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$AC$2</c:f>
+              <c:f>Salary!$B$2:$AC$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
@@ -1097,7 +1128,497 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Rank!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Rank!$B$1:$AE$1</c:f>
+              <c:strCache>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>YEAR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SALARY</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AGE</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>W</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MIN</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PTS</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FGM</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FGA</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>FG%</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3PM</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3PA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3P%</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>FTM</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>FTA</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>FT%</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>OREB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>DREB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>REB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>AST</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>TOV</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>STL</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>BLK</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>PF</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>FP</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>DD2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>TD3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>+/-</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>RK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Rank!$B$2:$AE$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>-4.5077509999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.79920351000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.27972801000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.35598222499999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.30014096099999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.23401364199999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.64292019199999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.61148608100000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.60886937299999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.606308399</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.10952327100000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.44612375999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.46446205800000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.25266329199999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.52274076700000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.51630252399999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.20109032900000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.16320976200000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.49380512599999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.42925624499999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.49665182600000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.57427726599999995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.493858405</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.20709322499999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.42768297199999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.62894778200000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.37607540099999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.22859185500000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.22939609999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C594-4168-AD4A-2510E5AFB3D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1749445343"/>
+        <c:axId val="1749478975"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1749445343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1749478975"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1749478975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1749445343"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1640,18 +2161,521 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1562100</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>577850</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
@@ -1661,6 +2685,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{312964FE-0C92-422E-BDA6-7989147E3873}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EABB745-381B-48B9-9F3E-B442C0442981}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1981,7 +3046,7 @@
   <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="A3" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4949,13 +6014,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C322C98-A926-4600-BFE0-777ECF8C4FDC}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
@@ -5150,4 +6215,219 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5474815F-6916-4B8E-9600-12ECBE75F33A}">
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>-4.5077509999999999E-3</v>
+      </c>
+      <c r="C2">
+        <v>-0.79920351000000001</v>
+      </c>
+      <c r="D2">
+        <v>-0.27972801000000003</v>
+      </c>
+      <c r="E2">
+        <v>-0.35598222499999999</v>
+      </c>
+      <c r="F2">
+        <v>-0.30014096099999998</v>
+      </c>
+      <c r="G2">
+        <v>-0.23401364199999999</v>
+      </c>
+      <c r="H2">
+        <v>-0.64292019199999995</v>
+      </c>
+      <c r="I2">
+        <v>-0.61148608100000001</v>
+      </c>
+      <c r="J2">
+        <v>-0.60886937299999999</v>
+      </c>
+      <c r="K2">
+        <v>-0.606308399</v>
+      </c>
+      <c r="L2">
+        <v>-0.10952327100000001</v>
+      </c>
+      <c r="M2">
+        <v>-0.44612375999999998</v>
+      </c>
+      <c r="N2">
+        <v>-0.46446205800000001</v>
+      </c>
+      <c r="O2">
+        <v>-0.25266329199999998</v>
+      </c>
+      <c r="P2">
+        <v>-0.52274076700000005</v>
+      </c>
+      <c r="Q2">
+        <v>-0.51630252399999998</v>
+      </c>
+      <c r="R2">
+        <v>-0.20109032900000001</v>
+      </c>
+      <c r="S2">
+        <v>-0.16320976200000001</v>
+      </c>
+      <c r="T2">
+        <v>-0.49380512599999998</v>
+      </c>
+      <c r="U2">
+        <v>-0.42925624499999998</v>
+      </c>
+      <c r="V2">
+        <v>-0.49665182600000002</v>
+      </c>
+      <c r="W2">
+        <v>-0.57427726599999995</v>
+      </c>
+      <c r="X2">
+        <v>-0.493858405</v>
+      </c>
+      <c r="Y2">
+        <v>-0.20709322499999999</v>
+      </c>
+      <c r="Z2">
+        <v>-0.42768297199999999</v>
+      </c>
+      <c r="AA2">
+        <v>-0.62894778200000001</v>
+      </c>
+      <c r="AB2">
+        <v>-0.37607540099999998</v>
+      </c>
+      <c r="AC2">
+        <v>-0.22859185500000001</v>
+      </c>
+      <c r="AD2">
+        <v>-0.22939609999999999</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD2">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="-0.5"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>